<commit_message>
Added js to populate field dropdown on change of category dropdown
</commit_message>
<xml_diff>
--- a/docs/BaseReportCriteria.xlsx
+++ b/docs/BaseReportCriteria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\TelefunkenU87\Practitioner\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E05425-2902-4007-9377-6E9B2F6E3F51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D30D01-FD3F-487E-B565-F7F47AA0D15D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{49BF3104-0EF2-4885-A594-DD7F815DDCAB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="87">
   <si>
     <t>Demographics</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>Category</t>
+  </si>
+  <si>
+    <t>BaseReportCriteriaId</t>
   </si>
 </sst>
 </file>
@@ -642,467 +645,590 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C366FD16-E888-4CF0-8687-9EC9226C9464}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="2" max="2" width="36.77734375" customWidth="1"/>
-    <col min="3" max="3" width="30.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="36.77734375" customWidth="1"/>
+    <col min="4" max="4" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
         <v>85</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>83</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>0</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>0</v>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>0</v>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>0</v>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>0</v>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>0</v>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>0</v>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>0</v>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>0</v>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>0</v>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>0</v>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
         <v>28</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>0</v>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
         <v>29</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>0</v>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
         <v>30</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>31</v>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
         <v>38</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>31</v>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
         <v>39</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>31</v>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
         <v>42</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>31</v>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
         <v>43</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>31</v>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
         <v>40</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>31</v>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
         <v>41</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>31</v>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
         <v>51</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>31</v>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
         <v>52</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>31</v>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
         <v>53</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>31</v>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" t="s">
         <v>54</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>31</v>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
         <v>55</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>31</v>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" t="s">
         <v>56</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>31</v>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" t="s">
         <v>57</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>31</v>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" t="s">
         <v>61</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>31</v>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" t="s">
         <v>62</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
         <v>63</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
         <v>64</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>70</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
         <v>64</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>71</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
         <v>64</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>72</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
         <v>64</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>73</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
         <v>64</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>74</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
         <v>64</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>76</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
         <v>64</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>78</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
         <v>64</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>81</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
         <v>64</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>82</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Selects distinct values after selecting a field in reports criteria
</commit_message>
<xml_diff>
--- a/docs/BaseReportCriteria.xlsx
+++ b/docs/BaseReportCriteria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\TelefunkenU87\Practitioner\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D30D01-FD3F-487E-B565-F7F47AA0D15D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B7CBC1-511F-42BA-9EA9-D3FAAA7A2506}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{49BF3104-0EF2-4885-A594-DD7F815DDCAB}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="16440" windowHeight="9420" xr2:uid="{49BF3104-0EF2-4885-A594-DD7F815DDCAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="95">
   <si>
     <t>Demographics</t>
   </si>
@@ -294,6 +294,30 @@
   </si>
   <si>
     <t>BaseReportCriteriaId</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>AccountServed</t>
+  </si>
+  <si>
+    <t>PracticeManagement</t>
+  </si>
+  <si>
+    <t>BoardsCommittees</t>
+  </si>
+  <si>
+    <t>CareerInterest</t>
+  </si>
+  <si>
+    <t>GeneralInterest</t>
+  </si>
+  <si>
+    <t>ReloInterest</t>
+  </si>
+  <si>
+    <t>SourceTable</t>
   </si>
 </sst>
 </file>
@@ -645,20 +669,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C366FD16-E888-4CF0-8687-9EC9226C9464}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="36.77734375" customWidth="1"/>
-    <col min="4" max="4" width="30.77734375" customWidth="1"/>
+    <col min="3" max="4" width="36.77734375" customWidth="1"/>
+    <col min="5" max="5" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>86</v>
       </c>
@@ -669,10 +693,13 @@
         <v>83</v>
       </c>
       <c r="D1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -683,10 +710,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -697,10 +727,13 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -711,10 +744,13 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -725,10 +761,13 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -739,10 +778,13 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -753,10 +795,13 @@
         <v>21</v>
       </c>
       <c r="D7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -767,10 +812,13 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -781,10 +829,13 @@
         <v>23</v>
       </c>
       <c r="D9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -795,10 +846,13 @@
         <v>24</v>
       </c>
       <c r="D10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -809,10 +863,13 @@
         <v>25</v>
       </c>
       <c r="D11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -823,10 +880,13 @@
         <v>26</v>
       </c>
       <c r="D12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -837,10 +897,13 @@
         <v>27</v>
       </c>
       <c r="D13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -851,10 +914,13 @@
         <v>28</v>
       </c>
       <c r="D14" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -865,10 +931,13 @@
         <v>29</v>
       </c>
       <c r="D15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -879,10 +948,13 @@
         <v>30</v>
       </c>
       <c r="D16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -893,10 +965,13 @@
         <v>38</v>
       </c>
       <c r="D17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -907,10 +982,13 @@
         <v>39</v>
       </c>
       <c r="D18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -921,10 +999,13 @@
         <v>42</v>
       </c>
       <c r="D19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -935,10 +1016,13 @@
         <v>43</v>
       </c>
       <c r="D20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -949,10 +1033,13 @@
         <v>40</v>
       </c>
       <c r="D21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -963,10 +1050,13 @@
         <v>41</v>
       </c>
       <c r="D22" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -977,10 +1067,13 @@
         <v>51</v>
       </c>
       <c r="D23" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -991,10 +1084,13 @@
         <v>52</v>
       </c>
       <c r="D24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1005,10 +1101,13 @@
         <v>53</v>
       </c>
       <c r="D25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1019,10 +1118,13 @@
         <v>54</v>
       </c>
       <c r="D26" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1033,10 +1135,13 @@
         <v>55</v>
       </c>
       <c r="D27" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1047,10 +1152,13 @@
         <v>56</v>
       </c>
       <c r="D28" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1061,10 +1169,13 @@
         <v>57</v>
       </c>
       <c r="D29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1075,10 +1186,13 @@
         <v>61</v>
       </c>
       <c r="D30" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1089,10 +1203,13 @@
         <v>62</v>
       </c>
       <c r="D31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1103,10 +1220,13 @@
         <v>63</v>
       </c>
       <c r="D32" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1117,10 +1237,13 @@
         <v>70</v>
       </c>
       <c r="D33" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1131,10 +1254,13 @@
         <v>71</v>
       </c>
       <c r="D34" t="s">
+        <v>91</v>
+      </c>
+      <c r="E34" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1145,10 +1271,13 @@
         <v>72</v>
       </c>
       <c r="D35" t="s">
+        <v>91</v>
+      </c>
+      <c r="E35" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1159,10 +1288,13 @@
         <v>73</v>
       </c>
       <c r="D36" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1173,10 +1305,13 @@
         <v>74</v>
       </c>
       <c r="D37" t="s">
+        <v>91</v>
+      </c>
+      <c r="E37" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1187,10 +1322,13 @@
         <v>76</v>
       </c>
       <c r="D38" t="s">
+        <v>92</v>
+      </c>
+      <c r="E38" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1201,10 +1339,13 @@
         <v>78</v>
       </c>
       <c r="D39" t="s">
+        <v>93</v>
+      </c>
+      <c r="E39" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1215,10 +1356,13 @@
         <v>81</v>
       </c>
       <c r="D40" t="s">
+        <v>93</v>
+      </c>
+      <c r="E40" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1229,6 +1373,9 @@
         <v>82</v>
       </c>
       <c r="D41" t="s">
+        <v>93</v>
+      </c>
+      <c r="E41" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>